<commit_message>
add get fast result with tables
</commit_message>
<xml_diff>
--- a/img_for_ui/Сводная_таблица_по_месторождениям.xlsx
+++ b/img_for_ui/Сводная_таблица_по_месторождениям.xlsx
@@ -5,20 +5,21 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\for made\Pycharm-projects\Unstructured-field-data-aggregator\get_result\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\for made\Pycharm-projects\Unstructured-field-data-aggregator\img_for_ui\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57D1FDDB-0C5E-487C-B9F2-F013AC3D0433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B42646-B828-4B54-AB40-B701EE775327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{A0528918-EE30-4AB7-8895-26226FBF2744}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="9960" firstSheet="2" activeTab="5" xr2:uid="{A0528918-EE30-4AB7-8895-26226FBF2744}"/>
   </bookViews>
   <sheets>
     <sheet name="Архангельское" sheetId="1" r:id="rId1"/>
-    <sheet name="Матросовское" sheetId="8" r:id="rId2"/>
-    <sheet name="Ивинское" sheetId="5" r:id="rId3"/>
-    <sheet name="Граничное" sheetId="3" r:id="rId4"/>
-    <sheet name="Байданкинское" sheetId="6" r:id="rId5"/>
-    <sheet name="Щербенское" sheetId="7" r:id="rId6"/>
+    <sheet name="Аканское" sheetId="9" r:id="rId2"/>
+    <sheet name="Матросовское" sheetId="8" r:id="rId3"/>
+    <sheet name="Ивинское" sheetId="5" r:id="rId4"/>
+    <sheet name="Граничное" sheetId="3" r:id="rId5"/>
+    <sheet name="Байданкинское" sheetId="6" r:id="rId6"/>
+    <sheet name="Щербенское" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="84">
   <si>
     <t>объекты</t>
   </si>
@@ -291,6 +292,9 @@
   <si>
     <t>0,464;
 0,300 (СВН)</t>
+  </si>
+  <si>
+    <t>Аканское месторождение</t>
   </si>
 </sst>
 </file>
@@ -422,7 +426,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -487,24 +491,22 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -822,8 +824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{256C3014-DB5B-4831-B1EC-5C0F03C703CF}">
   <dimension ref="A1:T50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="116" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B10"/>
+    <sheetView topLeftCell="B1" zoomScale="69" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C12" sqref="A1:R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -897,22 +899,22 @@
       <c r="R1" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="T1" s="28"/>
+      <c r="T1" s="7"/>
     </row>
     <row r="2" spans="1:20" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="25" t="s">
         <v>42</v>
       </c>
       <c r="F2" s="15" t="s">
@@ -954,14 +956,13 @@
       <c r="R2" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="T2" s="29"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A3" s="27"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
+      <c r="A3" s="25"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
       <c r="F3" s="15" t="s">
         <v>3</v>
       </c>
@@ -1001,14 +1002,13 @@
       <c r="R3" s="16">
         <v>0</v>
       </c>
-      <c r="T3" s="29"/>
     </row>
     <row r="4" spans="1:20" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="27"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
       <c r="F4" s="15" t="s">
         <v>4</v>
       </c>
@@ -1048,14 +1048,13 @@
       <c r="R4" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="T4" s="29"/>
     </row>
     <row r="5" spans="1:20" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="27"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
+      <c r="A5" s="25"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
       <c r="F5" s="15" t="s">
         <v>5</v>
       </c>
@@ -1095,14 +1094,13 @@
       <c r="R5" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="T5" s="29"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A6" s="27"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
       <c r="F6" s="15" t="s">
         <v>6</v>
       </c>
@@ -1142,14 +1140,13 @@
       <c r="R6" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="T6" s="29"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A7" s="27"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
+      <c r="A7" s="25"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
       <c r="F7" s="15" t="s">
         <v>7</v>
       </c>
@@ -1189,14 +1186,13 @@
       <c r="R7" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="T7" s="29"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A8" s="27"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
+      <c r="A8" s="25"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
       <c r="F8" s="15" t="s">
         <v>8</v>
       </c>
@@ -1236,14 +1232,13 @@
       <c r="R8" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="T8" s="29"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A9" s="27"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
+      <c r="A9" s="25"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
       <c r="F9" s="15" t="s">
         <v>9</v>
       </c>
@@ -1283,14 +1278,13 @@
       <c r="R9" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="T9" s="29"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A10" s="27"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
       <c r="F10" s="15" t="s">
         <v>11</v>
       </c>
@@ -1330,18 +1324,17 @@
       <c r="R10" s="16">
         <v>4</v>
       </c>
-      <c r="T10" s="29"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="24" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A12" s="26"/>
+      <c r="A12" s="27"/>
       <c r="B12" s="4" t="s">
         <v>59</v>
       </c>
@@ -1441,98 +1434,33 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A410D37C-2141-43C2-AF8B-50084372A8CE}">
-  <dimension ref="A1:K4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F226E67B-5A43-487F-B6AE-7B189F662390}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="82" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.21875" customWidth="1"/>
-    <col min="2" max="2" width="34.88671875" customWidth="1"/>
-    <col min="3" max="3" width="31.6640625" customWidth="1"/>
-    <col min="4" max="4" width="30.33203125" customWidth="1"/>
-    <col min="5" max="5" width="74.44140625" customWidth="1"/>
-    <col min="6" max="6" width="25.44140625" customWidth="1"/>
-    <col min="7" max="7" width="18.5546875" customWidth="1"/>
-    <col min="9" max="9" width="25.5546875" customWidth="1"/>
-    <col min="10" max="10" width="14.33203125" customWidth="1"/>
+    <col min="1" max="1" width="25.44140625" customWidth="1"/>
+    <col min="2" max="2" width="38.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="4"/>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="4">
-        <v>3</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="4">
-        <v>0.61</v>
-      </c>
-      <c r="J2" s="4">
-        <v>0.06</v>
-      </c>
-      <c r="K2" s="4">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B4" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>60</v>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1541,11 +1469,108 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A410D37C-2141-43C2-AF8B-50084372A8CE}">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView zoomScale="82" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="34.88671875" customWidth="1"/>
+    <col min="2" max="2" width="31.6640625" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" customWidth="1"/>
+    <col min="4" max="4" width="74.44140625" customWidth="1"/>
+    <col min="5" max="5" width="25.44140625" customWidth="1"/>
+    <col min="6" max="6" width="18.5546875" customWidth="1"/>
+    <col min="8" max="8" width="25.5546875" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="4">
+        <v>3</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="4">
+        <v>0.61</v>
+      </c>
+      <c r="I2" s="4">
+        <v>0.06</v>
+      </c>
+      <c r="J2" s="4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C492253F-F25E-4619-A849-DA0F3433CDB4}">
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E7"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1693,12 +1718,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEA6B032-E062-4BBA-B6CB-393B01DCC477}">
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView zoomScale="116" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D8" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1818,12 +1843,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE3E4C29-4286-4F96-ACE4-C6F6B6FC4AC5}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView zoomScale="104" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="104" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C19" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1864,16 +1889,16 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="28" t="s">
         <v>71</v>
       </c>
       <c r="E2" s="4" t="s">
@@ -1888,10 +1913,10 @@
       <c r="H2" s="4"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="25"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="24"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="28"/>
       <c r="E3" s="4" t="s">
         <v>5</v>
       </c>
@@ -1974,12 +1999,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D071E582-4619-4083-96AC-3B220330E423}">
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView zoomScale="117" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>